<commit_message>
26 05 2023 1
</commit_message>
<xml_diff>
--- a/krilov/files/22/22var20.xlsx
+++ b/krilov/files/22/22var20.xlsx
@@ -4,11 +4,43 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Лист1!$K$5</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Лист1!$B$8</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$K$7</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID процесса B</t>
   </si>
@@ -34,9 +66,6 @@
   </si>
   <si>
     <t>8; 9; 10; 11</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
 </sst>
 </file>
@@ -53,12 +82,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -347,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -358,14 +395,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -389,7 +426,7 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>5</v>
       </c>
     </row>
@@ -403,7 +440,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>B3+D2</f>
         <v>10</v>
       </c>
@@ -418,7 +455,7 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>B4</f>
         <v>3</v>
       </c>
@@ -433,7 +470,7 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f>B5+D4</f>
         <v>5</v>
       </c>
@@ -448,8 +485,8 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <f>B6+D3</f>
+      <c r="D6" s="2">
+        <f>B6+ MAX(D3,D5)</f>
         <v>14</v>
       </c>
     </row>
@@ -463,7 +500,7 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f>B7</f>
         <v>1</v>
       </c>
@@ -472,13 +509,14 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
+      <c r="B8" s="1">
+        <v>4</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
+        <f>B8+D7</f>
         <v>5</v>
       </c>
     </row>
@@ -492,8 +530,9 @@
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>6</v>
+      <c r="D9" s="2">
+        <f>B9+D8</f>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,7 +545,7 @@
       <c r="C10">
         <v>6</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f>B10+D7</f>
         <v>6</v>
       </c>
@@ -521,7 +560,7 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f>B11</f>
         <v>3</v>
       </c>
@@ -536,7 +575,7 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <f>B12</f>
         <v>5</v>
       </c>
@@ -551,8 +590,9 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13">
-        <v>14</v>
+      <c r="D13" s="2">
+        <f>B13+MAX(D9:D11)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>